<commit_message>
added updated data sept 6
</commit_message>
<xml_diff>
--- a/data/DengueCaseReporting[2012-23].xlsx
+++ b/data/DengueCaseReporting[2012-23].xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\01 Projects\Dashboards\dengue-situation-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5538338A-0EB5-446C-883B-71C8001DCC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9AE0A-F4FA-44FF-B6CC-006EFF7ED94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1605" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,7 +368,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -780,7 +780,7 @@
         <v>9911</v>
       </c>
       <c r="M10" s="4">
-        <v>12108</v>
+        <v>14214</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -916,7 +916,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1238,7 @@
         <v>34</v>
       </c>
       <c r="J10" s="4">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added all the changes
</commit_message>
<xml_diff>
--- a/data/DengueCaseReporting[2012-23].xlsx
+++ b/data/DengueCaseReporting[2012-23].xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\01 Projects\Dashboards\dengue-situation-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9AE0A-F4FA-44FF-B6CC-006EFF7ED94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD516CB7-89B0-441A-B786-BA70ACE8C2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1605" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dengue Cases 2012-2023" sheetId="1" r:id="rId1"/>
@@ -90,6 +90,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -367,8 +368,8 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -780,7 +781,7 @@
         <v>9911</v>
       </c>
       <c r="M10" s="4">
-        <v>14214</v>
+        <v>21527</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -915,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C434D647-C904-4EBE-9056-3E9E700EC43C}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1239,7 @@
         <v>34</v>
       </c>
       <c r="J10" s="4">
-        <v>78</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added sept 11 data
</commit_message>
<xml_diff>
--- a/data/DengueCaseReporting[2012-23].xlsx
+++ b/data/DengueCaseReporting[2012-23].xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\01 Projects\Dashboards\dengue-situation-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD516CB7-89B0-441A-B786-BA70ACE8C2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49139A72-502D-4E1F-952F-3132856979B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dengue Cases 2012-2023" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
@@ -781,7 +781,7 @@
         <v>9911</v>
       </c>
       <c r="M10" s="4">
-        <v>21527</v>
+        <v>27464</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C434D647-C904-4EBE-9056-3E9E700EC43C}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1239,7 +1239,7 @@
         <v>34</v>
       </c>
       <c r="J10" s="4">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>